<commit_message>
Added new project for second PCIe interface
</commit_message>
<xml_diff>
--- a/Documents/BOM.xlsx
+++ b/Documents/BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CC4514-4077-4BDC-BADA-2FF04B781EDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C649E7C-554D-4878-B112-C4C48339DD04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2100" windowWidth="38640" windowHeight="21240" tabRatio="951" xr2:uid="{D471A551-4AA1-4241-A607-672352FF3AE8}"/>
+    <workbookView xWindow="-38400" yWindow="-1620" windowWidth="38400" windowHeight="19620" tabRatio="951" xr2:uid="{D471A551-4AA1-4241-A607-672352FF3AE8}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="14" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
   <si>
     <t>Description</t>
   </si>
@@ -127,9 +127,6 @@
     <t>9DBV0441</t>
   </si>
   <si>
-    <t>PCIe clock distribution</t>
-  </si>
-  <si>
     <t>I2C I/O expander</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>Unknown PCIe card</t>
   </si>
   <si>
-    <t>U5825IMY</t>
-  </si>
-  <si>
     <t>000193 ACP022 1545</t>
   </si>
   <si>
@@ -341,6 +335,21 @@
   </si>
   <si>
     <t>12 MHz For FT232H</t>
+  </si>
+  <si>
+    <t>9DBV0241</t>
+  </si>
+  <si>
+    <t>4-Output 1.8V PCIe Fanout Buffer</t>
+  </si>
+  <si>
+    <t>2-Output 1.8V PCIe Fanout Buffer</t>
+  </si>
+  <si>
+    <t>PCIe clock distribution (OCP card)</t>
+  </si>
+  <si>
+    <t>PCIe clock distribution (PCIe card)</t>
   </si>
 </sst>
 </file>
@@ -584,7 +593,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -613,24 +622,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -675,47 +666,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -728,66 +683,117 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1117,14 +1123,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="19" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1138,11 +1144,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>32</v>
@@ -1150,445 +1156,447 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="66" t="s">
+      <c r="A3" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="B3" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="12"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="41" t="s">
+      <c r="C6" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="49"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="63"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="50"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="42"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="41" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="51" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="43"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="31"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="31"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B23" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="71"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
-      <c r="B19" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="38" t="s">
+      <c r="C23" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="53"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>82</v>
+      <c r="B25" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="57"/>
-      <c r="B26" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="49" t="s">
-        <v>83</v>
+      <c r="B26" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="55"/>
+      <c r="D26" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="49" t="s">
-        <v>104</v>
+      <c r="B27" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="31" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="49" t="s">
-        <v>103</v>
+      <c r="B28" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="31" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="49" t="s">
-        <v>102</v>
+      <c r="B29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="55"/>
+      <c r="D29" s="31" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="49" t="s">
-        <v>101</v>
+      <c r="B30" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="55"/>
+      <c r="D30" s="31" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="49" t="s">
-        <v>100</v>
+      <c r="B31" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="55"/>
+      <c r="D31" s="31" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="57"/>
-      <c r="B32" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="49" t="s">
-        <v>99</v>
+      <c r="B32" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="55"/>
+      <c r="D32" s="31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="49" t="s">
-        <v>98</v>
+      <c r="B33" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="55"/>
+      <c r="D33" s="31" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="49" t="s">
-        <v>97</v>
+      <c r="B34" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="55"/>
+      <c r="D34" s="31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="59" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="60" t="s">
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="53"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
@@ -1596,20 +1604,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C34"/>
-    <mergeCell ref="A31:A32"/>
+  <mergeCells count="20">
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A5:A6"/>
@@ -1618,6 +1614,17 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C13:C15"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C34"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>